<commit_message>
Move Question 96 from Audit report group to Year-End report group.
This was an error in the grouping data so it regenerates the data
files as well.
</commit_message>
<xml_diff>
--- a/data/GroupingsOBSQuestions2015.xlsx
+++ b/data/GroupingsOBSQuestions2015.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="QuestionsGroups" sheetId="1" state="visible" r:id="rId2"/>
@@ -87,13 +87,13 @@
     <t>Year-End Report</t>
   </si>
   <si>
-    <t>84-95, 139</t>
+    <t>84-96, 139</t>
   </si>
   <si>
     <t>Audit Report</t>
   </si>
   <si>
-    <t>96-102, 140</t>
+    <t>97-102, 140</t>
   </si>
   <si>
     <t>Info throughout all eight key documents</t>
@@ -672,13 +672,13 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.83400809716599"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.83400809716599"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.8265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.8265306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -731,6 +731,9 @@
         <v>7</v>
       </c>
     </row>
+    <row r="7" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0"/>
+    </row>
     <row r="8" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0"/>
       <c r="B8" s="4" t="s">
@@ -827,6 +830,9 @@
       <c r="C16" s="5" t="s">
         <v>25</v>
       </c>
+    </row>
+    <row r="17" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0"/>
@@ -902,8 +908,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1023" min="1" style="5" width="8.83400809716599"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.83400809716599"/>
+    <col collapsed="false" hidden="false" max="1023" min="1" style="5" width="8.8265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.8265306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>